<commit_message>
- First Release - Pending:     1. Ltp calculation using main broker     2. Stylesheet change at positions screen group-by window
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="53">
   <si>
     <t xml:space="preserve">transaction_type</t>
   </si>
@@ -121,9 +121,6 @@
     <t xml:space="preserve">Sell</t>
   </si>
   <si>
-    <t xml:space="preserve">0.0</t>
-  </si>
-  <si>
     <t xml:space="preserve">LIMIT</t>
   </si>
   <si>
@@ -142,7 +139,7 @@
     <t xml:space="preserve">2022-03-17</t>
   </si>
   <si>
-    <t xml:space="preserve">ATM+4 CE</t>
+    <t xml:space="preserve">ATM CE</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -154,16 +151,13 @@
     <t xml:space="preserve">Value</t>
   </si>
   <si>
-    <t xml:space="preserve">10</t>
-  </si>
-  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
     <t xml:space="preserve">NO</t>
   </si>
   <si>
-    <t xml:space="preserve">NEW</t>
+    <t xml:space="preserve">new</t>
   </si>
   <si>
     <t xml:space="preserve">21</t>
@@ -172,10 +166,19 @@
     <t xml:space="preserve">3</t>
   </si>
   <si>
-    <t xml:space="preserve">NIFTY2231717000CE</t>
+    <t xml:space="preserve">existing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIFTY2231717500CE</t>
   </si>
   <si>
     <t xml:space="preserve">Default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NIFTY2231716500PE</t>
   </si>
 </sst>
 </file>
@@ -251,17 +254,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -281,208 +280,523 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF2"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE2" activeCellId="0" sqref="AE2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AD1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE3" activeCellId="0" sqref="AE3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55859375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="9.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="15.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="10.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="21.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="15.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="18.89"/>
+  </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="0" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="S1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="U1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="V1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="W1" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="X1" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Y1" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="Z1" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AA1" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AC1" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="0" t="s">
         <v>29</v>
       </c>
       <c r="AE1" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AF1" s="0" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D2" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="E2" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R2" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="T2" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z2" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB2" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC2" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE2" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF2" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E3" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F3" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G3" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H3" s="0" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I3" s="0" t="s">
         <v>38</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J3" s="0" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="O2" s="1" t="s">
+      <c r="K3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="P3" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="T3" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U3" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="V3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="W3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="X3" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z3" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA3" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB3" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC3" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD3" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF3" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="P4" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R4" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="T4" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U4" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="S2" s="1" t="s">
+      <c r="V4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="W4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="X4" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z4" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA4" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB4" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC4" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AF4" s="0" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="N5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="Q5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="R5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="S5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="U5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="V5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="W5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="X5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="Y5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="Z5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="1" t="s">
+      <c r="AA5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="Z2" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE2" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AF2" s="1" t="s">
-        <v>51</v>
+      <c r="AB5" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="AC5" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AF5" s="0" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Optimized imports for app_data.py, main.py + Model__PositionsGrouping.py grouping issue fixed for proxy data + Added freeze support to main.py + Added logging in Model OMS, and updated process to check the checklist + OrderManagerTable.py updated type hints + TradingSymbolMapping.py updated 'ATR TS Multiplier' data type as float (astype usage)
*Multi-accounts order placement working (except iifl)
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -2,43 +2,27 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <charset val="1"/>
       <family val="2"/>
       <color rgb="FF000000"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="0"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,33 +42,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general" vertical="bottom"/>
-    </xf>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -441,40 +409,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr filterMode="0">
+  <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr fitToPage="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE1"/>
+  <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="S1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE1" activeCellId="0" sqref="AE1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.55859375" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col width="15.26" customWidth="1" style="1" min="1" max="1"/>
-    <col width="14.81" customWidth="1" style="1" min="2" max="2"/>
-    <col width="14.37" customWidth="1" style="1" min="3" max="3"/>
-    <col width="12.33" customWidth="1" style="1" min="5" max="5"/>
-    <col width="9.44" customWidth="1" style="1" min="7" max="7"/>
-    <col width="12.89" customWidth="1" style="1" min="8" max="8"/>
-    <col width="11.22" customWidth="1" style="1" min="9" max="9"/>
+    <col width="15.21875" customWidth="1" style="1" min="1" max="1"/>
+    <col width="14.77734375" customWidth="1" style="1" min="2" max="2"/>
+    <col width="14.33203125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="12.33203125" customWidth="1" style="1" min="5" max="5"/>
+    <col width="9.44140625" customWidth="1" style="1" min="7" max="7"/>
+    <col width="12.88671875" customWidth="1" style="1" min="8" max="8"/>
+    <col width="11.21875" customWidth="1" style="1" min="9" max="9"/>
     <col width="10" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.22" customWidth="1" style="1" min="14" max="14"/>
-    <col width="12.66" customWidth="1" style="1" min="15" max="15"/>
+    <col width="11.21875" customWidth="1" style="1" min="14" max="14"/>
+    <col width="12.6640625" customWidth="1" style="1" min="15" max="15"/>
     <col width="11" customWidth="1" style="1" min="19" max="19"/>
-    <col width="11.44" customWidth="1" style="1" min="23" max="23"/>
-    <col width="12.66" customWidth="1" style="1" min="25" max="25"/>
-    <col width="15.26" customWidth="1" style="1" min="26" max="26"/>
-    <col width="10.96" customWidth="1" style="1" min="27" max="27"/>
-    <col width="21.31" customWidth="1" style="1" min="28" max="28"/>
-    <col width="15.14" customWidth="1" style="1" min="29" max="29"/>
-    <col width="20.98" customWidth="1" style="1" min="30" max="30"/>
-    <col width="9.140000000000001" customWidth="1" style="1" min="1024" max="1024"/>
+    <col width="11.44140625" customWidth="1" style="1" min="23" max="23"/>
+    <col width="12.6640625" customWidth="1" style="1" min="25" max="25"/>
+    <col width="15.21875" customWidth="1" style="1" min="26" max="26"/>
+    <col width="11" customWidth="1" style="1" min="27" max="27"/>
+    <col width="21.33203125" customWidth="1" style="1" min="28" max="28"/>
+    <col width="15.109375" customWidth="1" style="1" min="29" max="29"/>
+    <col width="21" customWidth="1" style="1" min="30" max="30"/>
+    <col width="9.109375" customWidth="1" style="1" min="1024" max="1024"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="2">
+    <row r="1" ht="13.8" customHeight="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>transaction_type</t>
@@ -628,12 +596,325 @@
       <c r="AE1" t="inlineStr">
         <is>
           <t>strategy_name</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>MIS</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2022-04-07</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>NIFTY2240718050CE</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Y2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Z2" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="AA2" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AB2" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AD2" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AE2" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>0.0</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>MARKET</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>MIS</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>5.0</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>NFO</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>NIFTY</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2022-04-07</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>NIFTY2240718050PE</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="Y3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="Z3" t="inlineStr">
+        <is>
+          <t>1.7</t>
+        </is>
+      </c>
+      <c r="AA3" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AB3" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="AD3" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="AE3" t="inlineStr">
+        <is>
+          <t>Default</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="0" useFirstPageNumber="0" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup orientation="portrait" paperSize="9" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ File clean ups and added some debug statements need to remove, main_strategy.py: remaining exit order issues + updated gitignore to ignore all csv files
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -647,7 +647,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2240718050CE</t>
+          <t>NIFTY2240717750CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -677,7 +677,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
@@ -687,7 +687,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -697,7 +697,7 @@
       </c>
       <c r="T2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="U2" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
@@ -804,7 +804,7 @@
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NIFTY2240718050PE</t>
+          <t>NIFTY2240717750PE</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -834,7 +834,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>3</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
@@ -844,7 +844,7 @@
       </c>
       <c r="R3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1</t>
         </is>
       </c>
       <c r="S3" t="inlineStr">
@@ -854,7 +854,7 @@
       </c>
       <c r="T3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="U3" t="inlineStr">
@@ -884,7 +884,7 @@
       </c>
       <c r="Z3" t="inlineStr">
         <is>
-          <t>1.7</t>
+          <t>0.6</t>
         </is>
       </c>
       <c r="AA3" t="inlineStr">

</xml_diff>

<commit_message>
+ working code after cAsE issue is fixed + filter rejected orders of positions screen (pending)
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -642,12 +642,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-07</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2240717750CE</t>
+          <t>NIFTY2241318000CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>existing</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -759,7 +759,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -799,12 +799,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2022-04-07</t>
+          <t>2022-04-13</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NIFTY2240717750PE</t>
+          <t>NIFTY2241318000CE</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="AA3" t="inlineStr">
         <is>
-          <t>new</t>
+          <t>existing</t>
         </is>
       </c>
       <c r="AB3" t="inlineStr">

</xml_diff>

<commit_message>
+ TradeXCB with slicing. + OMS section clustered into 3 functions. + imports optimized for fast loading of application + Creation of positions file updated.
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -642,82 +642,82 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-13</t>
+          <t>2022-04-21</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2241318000CE</t>
+          <t>NIFTY2242117500CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>130</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="P2" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="U2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V2" t="inlineStr">
         <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="P2" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="R2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
+      <c r="W2" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="X2" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
       <c r="Y2" t="inlineStr">
@@ -799,12 +799,12 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2022-04-13</t>
+          <t>2022-04-21</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>NIFTY2241318000CE</t>
+          <t>NIFTY2242117500PE</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -819,62 +819,62 @@
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>150</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="P3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="U3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="V3" t="inlineStr">
+        <is>
           <t>NO</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
+      <c r="W3" t="inlineStr">
+        <is>
+          <t>new</t>
+        </is>
+      </c>
+      <c r="X3" t="inlineStr">
         <is>
           <t>NO</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>YES</t>
         </is>
       </c>
       <c r="Y3" t="inlineStr">

</xml_diff>

<commit_message>
+ Removed commented out codes from main_strategy.py + Separated custom_talib.py
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -2,14 +2,16 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -19,10 +21,10 @@
   <fonts count="1">
     <font>
       <name val="Calibri"/>
-      <charset val="1"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -45,14 +47,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -413,36 +414,33 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AE3"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
-  <cols>
-    <col width="15.21875" customWidth="1" style="1" min="1" max="1"/>
-    <col width="14.77734375" customWidth="1" style="1" min="2" max="2"/>
-    <col width="14.33203125" customWidth="1" style="1" min="3" max="3"/>
-    <col width="12.33203125" customWidth="1" style="1" min="5" max="5"/>
-    <col width="9.44140625" customWidth="1" style="1" min="7" max="7"/>
-    <col width="12.88671875" customWidth="1" style="1" min="8" max="8"/>
-    <col width="11.21875" customWidth="1" style="1" min="9" max="9"/>
-    <col width="10" customWidth="1" style="1" min="10" max="10"/>
-    <col width="11.21875" customWidth="1" style="1" min="14" max="14"/>
-    <col width="12.6640625" customWidth="1" style="1" min="15" max="15"/>
-    <col width="11" customWidth="1" style="1" min="19" max="19"/>
-    <col width="11.44140625" customWidth="1" style="1" min="23" max="23"/>
-    <col width="12.6640625" customWidth="1" style="1" min="25" max="25"/>
-    <col width="15.21875" customWidth="1" style="1" min="26" max="26"/>
-    <col width="11" customWidth="1" style="1" min="27" max="27"/>
-    <col width="21.33203125" customWidth="1" style="1" min="28" max="28"/>
-    <col width="15.109375" customWidth="1" style="1" min="29" max="29"/>
-    <col width="21" customWidth="1" style="1" min="30" max="30"/>
-    <col width="9.109375" customWidth="1" style="1" min="1024" max="1024"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" ht="13.8" customHeight="1" s="1">
+    <row r="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>transaction_type</t>
@@ -495,105 +493,40 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>buy_above</t>
+          <t>stoploss_type</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>use_priceba</t>
+          <t>stoploss</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>sell_below</t>
+          <t>tsl_type</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>use_pricesb</t>
+          <t>tsl</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>stoploss_type</t>
+          <t>target_type</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>stoploss</t>
+          <t>target</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>tsl_type</t>
+          <t>timeframe</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
-        <is>
-          <t>tsl</t>
-        </is>
-      </c>
-      <c r="S1" t="inlineStr">
-        <is>
-          <t>target_type</t>
-        </is>
-      </c>
-      <c r="T1" t="inlineStr">
-        <is>
-          <t>target</t>
-        </is>
-      </c>
-      <c r="U1" t="inlineStr">
-        <is>
-          <t>timeframe</t>
-        </is>
-      </c>
-      <c r="V1" t="inlineStr">
-        <is>
-          <t>vwap</t>
-        </is>
-      </c>
-      <c r="W1" t="inlineStr">
-        <is>
-          <t>vwap_signal</t>
-        </is>
-      </c>
-      <c r="X1" t="inlineStr">
-        <is>
-          <t>ATRTS</t>
-        </is>
-      </c>
-      <c r="Y1" t="inlineStr">
-        <is>
-          <t>ATR TS Period</t>
-        </is>
-      </c>
-      <c r="Z1" t="inlineStr">
-        <is>
-          <t>ATR TS Multiplier</t>
-        </is>
-      </c>
-      <c r="AA1" t="inlineStr">
-        <is>
-          <t>atrts_signal</t>
-        </is>
-      </c>
-      <c r="AB1" t="inlineStr">
-        <is>
-          <t>moving_average_period</t>
-        </is>
-      </c>
-      <c r="AC1" t="inlineStr">
-        <is>
-          <t>moving_average</t>
-        </is>
-      </c>
-      <c r="AD1" t="inlineStr">
-        <is>
-          <t>moving_average_signal</t>
-        </is>
-      </c>
-      <c r="AE1" t="inlineStr">
         <is>
           <t>strategy_name</t>
         </is>
@@ -602,7 +535,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -617,7 +550,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>MARKET</t>
+          <t>LIMIT</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -647,29 +580,29 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2242117500CE</t>
+          <t>NIFTY2242114350CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>130</t>
+          <t>Value</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>YES</t>
+          <t>0</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
+          <t>Value</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
       <c r="O2" t="inlineStr">
         <is>
           <t>Value</t>
@@ -677,244 +610,21 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>1</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U2" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="W2" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="X2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Z2" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="AA2" t="inlineStr">
-        <is>
-          <t>existing</t>
-        </is>
-      </c>
-      <c r="AB2" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AC2" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AD2" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="AE2" t="inlineStr">
-        <is>
-          <t>Default</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Sell</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0.0</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>MARKET</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>MIS</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>5.0</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>NFO</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>NIFTY</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>2022-04-21</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>NIFTY2242117500PE</t>
-        </is>
-      </c>
-      <c r="K3" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>150</t>
-        </is>
-      </c>
-      <c r="N3" t="inlineStr">
-        <is>
-          <t>YES</t>
-        </is>
-      </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="P3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="R3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="S3" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="T3" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
-      </c>
-      <c r="U3" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="V3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="W3" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="X3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="Z3" t="inlineStr">
-        <is>
-          <t>0.6</t>
-        </is>
-      </c>
-      <c r="AA3" t="inlineStr">
-        <is>
-          <t>existing</t>
-        </is>
-      </c>
-      <c r="AB3" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
-      </c>
-      <c r="AC3" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-      <c r="AD3" t="inlineStr">
-        <is>
-          <t>new</t>
-        </is>
-      </c>
-      <c r="AE3" t="inlineStr">
         <is>
           <t>Default</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup orientation="portrait" paperSize="9" firstPageNumber="0" horizontalDpi="300" verticalDpi="300"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ Code cleanup + Added new db username and password
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -535,7 +535,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -580,7 +580,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2242114350CE</t>
+          <t>NIFTY2242117250CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -590,7 +590,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -600,7 +600,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>2</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -610,12 +610,12 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>15</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>3</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">

</xml_diff>

<commit_message>
+ get_data raise ValueError on NoneType historical data + raise Exception on login failure + Updated orderbook logic, so that it doesn't show empty orders. + Deleted non-required files + Changed version to 0.1.7
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -575,12 +575,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-21</t>
+          <t>2022-04-28</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2242117250CE</t>
+          <t>NIFTY22APR17500CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>

<commit_message>
+ Updated time profiling code + Fixed slicing issue, where keeps on placing orders when n_slices > no. of lots
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -4,27 +4,42 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
+      <charset val="1"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="0"/>
+      <sz val="10"/>
     </font>
   </fonts>
   <fills count="2">
@@ -44,16 +59,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general" vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Percent" xfId="5" builtinId="5"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -410,37 +439,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="0" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr filterMode="0">
     <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M15" activeCellId="0" sqref="M15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="0" outlineLevelRow="0"/>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="15" customHeight="1" s="1">
       <c r="A1" t="inlineStr">
         <is>
           <t>transaction_type</t>
@@ -535,7 +566,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Buy</t>
+          <t>Sell</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -550,7 +581,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>LIMIT</t>
+          <t>MARKET</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -575,12 +606,12 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-04-28</t>
+          <t>2022-05-05</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY22APR17500CE</t>
+          <t>NIFTY2250517000CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -590,7 +621,7 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
@@ -600,7 +631,7 @@
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>5</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
@@ -610,12 +641,12 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>40</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>4</t>
         </is>
       </c>
       <c r="R2" t="inlineStr">
@@ -625,6 +656,8 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
+ Added import/export option in user api details. + Added load/export utilities in handle_user_details.py + Added color coding for non-required cells in User API details window. + Selection behaviour changed in API_Det_TableView.py + updated version to v0.1.9
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -566,7 +566,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sell</t>
+          <t>Buy</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2250517000CE</t>
+          <t>NIFTY2250517200PE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">

</xml_diff>

<commit_message>
+ Fixed issue in showing order status (3 functions changed) + Time profiling added for getting to close positions
</commit_message>
<xml_diff>
--- a/Libs/Files/DataFiles/tradexcb_strategy.xlsx
+++ b/Libs/Files/DataFiles/tradexcb_strategy.xlsx
@@ -606,29 +606,29 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2022-05-05</t>
+          <t>2022-05-12</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>NIFTY2250517200PE</t>
+          <t>NIFTY2251216000CE</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>Percentage</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>5</t>
@@ -636,7 +636,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Value</t>
+          <t>Percentage</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">

</xml_diff>